<commit_message>
update prizelist1 and fix EmpID from int to string
</commit_message>
<xml_diff>
--- a/prizelist1.xlsx
+++ b/prizelist1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarke\practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7304C074-2A56-490C-8880-A791FAE6DE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF7C0EE-055B-4542-84D9-EDE9F651658D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,13 +33,13 @@
     <t>Prize Name</t>
   </si>
   <si>
-    <t>Galaxy Buds2</t>
+    <t>Galaxy Buds R510F (BUDS 2 Pro)</t>
   </si>
   <si>
-    <t>Amazon voucher worth 3000</t>
+    <t>Amazon Vouchers NA 3000</t>
   </si>
   <si>
-    <t>Amazon voucher worth 2000</t>
+    <t>Amazon Vouchers NA 2000</t>
   </si>
 </sst>
 </file>
@@ -360,7 +360,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>